<commit_message>
new changes to the earliest assignments
</commit_message>
<xml_diff>
--- a/Exploring Excel/ProductionPivot_Solved.xlsx
+++ b/Exploring Excel/ProductionPivot_Solved.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cliffordboakyemensah/Netflix Bootcamp/NFLX-VIRT-DATA-PT-08-2021-E-LOL/02-Assignments/01-Introduction/01-Exploring_Plotting_Excel/Unsolved/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cliffordboakyemensah/BootCamp Assignments/Exploring Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{61D26620-9478-BE4F-9DD3-DA2823111813}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E2B88F4-F74F-A946-AB46-0F39FB8EAF17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="First Pivot" sheetId="3" r:id="rId1"/>
@@ -19,20 +19,12 @@
     <sheet name="Orders" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'Second Pivot'!$J$9</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'Second Pivot'!$J$9</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'Second Pivot'!$J$9</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'Second Pivot'!$J$9</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Orders!$H$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Orders!$H$2:$H$601</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Orders!$H$1</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Orders!$H$2:$H$601</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Orders!$H$1</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Orders!$H$2:$H$601</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Orders!$H$1</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Orders!$H$2:$H$601</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="9" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -52,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1237" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1302" uniqueCount="33">
   <si>
     <t>Product Name</t>
   </si>
@@ -302,40 +294,10 @@
   </mc:AlternateContent>
   <c:pivotSource>
     <c:name>[ProductionPivot_Solved.xlsx]Second Pivot!Shipping Priority Analysis</c:name>
-    <c:fmtId val="4"/>
+    <c:fmtId val="6"/>
   </c:pivotSource>
   <c:chart>
     <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Total Orders by Priority</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> for Biggest Proders</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -370,30 +332,16 @@
       <c:pivotFmt>
         <c:idx val="0"/>
         <c:spPr>
-          <a:ln w="28575" cap="rnd">
-            <a:solidFill>
-              <a:schemeClr val="accent2">
-                <a:lumMod val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="5"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln w="9525">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -440,8 +388,9 @@
     </c:pivotFmts>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="stacked"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -458,36 +407,20 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="75000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'Second Pivot'!$A$4:$A$24</c:f>
+              <c:f>'Second Pivot'!$A$4:$A$89</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="16"/>
+                <c:ptCount val="68"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>High</c:v>
@@ -537,19 +470,214 @@
                   <c:pt idx="15">
                     <c:v>VIP</c:v>
                   </c:pt>
+                  <c:pt idx="16">
+                    <c:v>High</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>Low</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>Medium</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>VIP</c:v>
+                  </c:pt>
+                  <c:pt idx="20">
+                    <c:v>High</c:v>
+                  </c:pt>
+                  <c:pt idx="21">
+                    <c:v>Low</c:v>
+                  </c:pt>
+                  <c:pt idx="22">
+                    <c:v>Medium</c:v>
+                  </c:pt>
+                  <c:pt idx="23">
+                    <c:v>VIP</c:v>
+                  </c:pt>
+                  <c:pt idx="24">
+                    <c:v>High</c:v>
+                  </c:pt>
+                  <c:pt idx="25">
+                    <c:v>Low</c:v>
+                  </c:pt>
+                  <c:pt idx="26">
+                    <c:v>Medium</c:v>
+                  </c:pt>
+                  <c:pt idx="27">
+                    <c:v>VIP</c:v>
+                  </c:pt>
+                  <c:pt idx="28">
+                    <c:v>High</c:v>
+                  </c:pt>
+                  <c:pt idx="29">
+                    <c:v>Low</c:v>
+                  </c:pt>
+                  <c:pt idx="30">
+                    <c:v>Medium</c:v>
+                  </c:pt>
+                  <c:pt idx="31">
+                    <c:v>VIP</c:v>
+                  </c:pt>
+                  <c:pt idx="32">
+                    <c:v>High</c:v>
+                  </c:pt>
+                  <c:pt idx="33">
+                    <c:v>Low</c:v>
+                  </c:pt>
+                  <c:pt idx="34">
+                    <c:v>Medium</c:v>
+                  </c:pt>
+                  <c:pt idx="35">
+                    <c:v>VIP</c:v>
+                  </c:pt>
+                  <c:pt idx="36">
+                    <c:v>High</c:v>
+                  </c:pt>
+                  <c:pt idx="37">
+                    <c:v>Low</c:v>
+                  </c:pt>
+                  <c:pt idx="38">
+                    <c:v>Medium</c:v>
+                  </c:pt>
+                  <c:pt idx="39">
+                    <c:v>VIP</c:v>
+                  </c:pt>
+                  <c:pt idx="40">
+                    <c:v>High</c:v>
+                  </c:pt>
+                  <c:pt idx="41">
+                    <c:v>Low</c:v>
+                  </c:pt>
+                  <c:pt idx="42">
+                    <c:v>Medium</c:v>
+                  </c:pt>
+                  <c:pt idx="43">
+                    <c:v>VIP</c:v>
+                  </c:pt>
+                  <c:pt idx="44">
+                    <c:v>High</c:v>
+                  </c:pt>
+                  <c:pt idx="45">
+                    <c:v>Low</c:v>
+                  </c:pt>
+                  <c:pt idx="46">
+                    <c:v>Medium</c:v>
+                  </c:pt>
+                  <c:pt idx="47">
+                    <c:v>VIP</c:v>
+                  </c:pt>
+                  <c:pt idx="48">
+                    <c:v>High</c:v>
+                  </c:pt>
+                  <c:pt idx="49">
+                    <c:v>Low</c:v>
+                  </c:pt>
+                  <c:pt idx="50">
+                    <c:v>Medium</c:v>
+                  </c:pt>
+                  <c:pt idx="51">
+                    <c:v>VIP</c:v>
+                  </c:pt>
+                  <c:pt idx="52">
+                    <c:v>High</c:v>
+                  </c:pt>
+                  <c:pt idx="53">
+                    <c:v>Low</c:v>
+                  </c:pt>
+                  <c:pt idx="54">
+                    <c:v>Medium</c:v>
+                  </c:pt>
+                  <c:pt idx="55">
+                    <c:v>VIP</c:v>
+                  </c:pt>
+                  <c:pt idx="56">
+                    <c:v>High</c:v>
+                  </c:pt>
+                  <c:pt idx="57">
+                    <c:v>Low</c:v>
+                  </c:pt>
+                  <c:pt idx="58">
+                    <c:v>Medium</c:v>
+                  </c:pt>
+                  <c:pt idx="59">
+                    <c:v>VIP</c:v>
+                  </c:pt>
+                  <c:pt idx="60">
+                    <c:v>High</c:v>
+                  </c:pt>
+                  <c:pt idx="61">
+                    <c:v>Low</c:v>
+                  </c:pt>
+                  <c:pt idx="62">
+                    <c:v>Medium</c:v>
+                  </c:pt>
+                  <c:pt idx="63">
+                    <c:v>VIP</c:v>
+                  </c:pt>
+                  <c:pt idx="64">
+                    <c:v>High</c:v>
+                  </c:pt>
+                  <c:pt idx="65">
+                    <c:v>Low</c:v>
+                  </c:pt>
+                  <c:pt idx="66">
+                    <c:v>Medium</c:v>
+                  </c:pt>
+                  <c:pt idx="67">
+                    <c:v>VIP</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
+                    <c:v>10 Foot HDMI Cable</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
                     <c:v>10 Foot USB Cable</c:v>
                   </c:pt>
-                  <c:pt idx="4">
+                  <c:pt idx="8">
+                    <c:v>128GB Flash Drive</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>16GB Flash Drive</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
                     <c:v>2 Foot USB Cable</c:v>
                   </c:pt>
-                  <c:pt idx="8">
+                  <c:pt idx="20">
+                    <c:v>32GB Flash Drive</c:v>
+                  </c:pt>
+                  <c:pt idx="24">
+                    <c:v>5 Foot HDMI Cable</c:v>
+                  </c:pt>
+                  <c:pt idx="28">
+                    <c:v>5 Foot USB Cable</c:v>
+                  </c:pt>
+                  <c:pt idx="32">
                     <c:v>64GB Flash Drive</c:v>
                   </c:pt>
-                  <c:pt idx="12">
+                  <c:pt idx="36">
+                    <c:v>Blue Ray DVD</c:v>
+                  </c:pt>
+                  <c:pt idx="40">
+                    <c:v>Bluetooth Keyboard</c:v>
+                  </c:pt>
+                  <c:pt idx="44">
+                    <c:v>Bluetooth Mouse</c:v>
+                  </c:pt>
+                  <c:pt idx="48">
+                    <c:v>Standard Edition DVD</c:v>
+                  </c:pt>
+                  <c:pt idx="52">
+                    <c:v>VHS Tape</c:v>
+                  </c:pt>
+                  <c:pt idx="56">
+                    <c:v>Wired Keyboard</c:v>
+                  </c:pt>
+                  <c:pt idx="60">
                     <c:v>Wired Mouse</c:v>
+                  </c:pt>
+                  <c:pt idx="64">
+                    <c:v>Wireless Router</c:v>
                   </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
@@ -557,65 +685,220 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Second Pivot'!$B$4:$B$24</c:f>
+              <c:f>'Second Pivot'!$B$4:$B$89</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="68"/>
                 <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="5">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="6">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="7">
                   <c:v>13</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="8">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="16">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="18">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="19">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="20">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="21">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="33">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="34">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="35">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="36">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="45">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="46">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="49">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="50">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="57">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="58">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="60">
                   <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-7502-2E41-A27D-C0D1B66C33C8}"/>
+              <c16:uniqueId val="{00000000-92F7-0D46-BCD3-DD855D74EBD9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -627,13 +910,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="510075840"/>
-        <c:axId val="510077488"/>
-      </c:lineChart>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1620128816"/>
+        <c:axId val="1620130720"/>
+      </c:barChart>
       <c:catAx>
-        <c:axId val="510075840"/>
+        <c:axId val="1620128816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -676,7 +959,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="510077488"/>
+        <c:crossAx val="1620130720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -684,7 +967,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="510077488"/>
+        <c:axId val="1620130720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -735,13 +1018,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="510075840"/>
+        <c:crossAx val="1620128816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="25400">
           <a:noFill/>
         </a:ln>
         <a:effectLst/>
@@ -779,7 +1062,7 @@
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="zero"/>
+    <c:dispBlanksAs val="gap"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -843,7 +1126,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.5</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -881,7 +1164,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{758B201C-8574-A840-A9FA-28EB4BAD892F}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.4</cx:f>
+              <cx:f>_xlchart.v1.0</cx:f>
               <cx:v>Total</cx:v>
             </cx:txData>
           </cx:tx>
@@ -989,7 +1272,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -2050,23 +2333,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>146050</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>660400</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 6">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ECD91410-5E1A-F94C-AF0A-7653A4B5CED5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0CBDF79-8830-6D47-8A79-FCA902EE31A4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8911,7 +9194,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0979E394-2C76-4546-B718-BE4674AC43D4}" name="PivotTable1" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0979E394-2C76-4546-B718-BE4674AC43D4}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A4:B11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField axis="axisRow" showAll="0">
@@ -9570,6 +9853,20 @@
     <dataField name="Count of Order Number" fld="1" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <conditionalFormats count="2">
+    <conditionalFormat priority="1">
+      <pivotAreas count="1">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="0" count="1">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
     <conditionalFormat priority="2">
       <pivotAreas count="1">
         <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
@@ -9589,20 +9886,6 @@
         </pivotArea>
       </pivotAreas>
     </conditionalFormat>
-    <conditionalFormat priority="1">
-      <pivotAreas count="1">
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="2">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="0" count="1">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
   </conditionalFormats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -9617,8 +9900,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{696DAC26-F4B7-DA44-B54E-47CC57454AB4}" name="Shipping Priority Analysis" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
-  <location ref="A3:B24" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{696DAC26-F4B7-DA44-B54E-47CC57454AB4}" name="Shipping Priority Analysis" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8">
+  <location ref="A3:B89" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0">
@@ -10227,7 +10510,7 @@
       </items>
     </pivotField>
     <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0" measureFilter="1">
+    <pivotField axis="axisRow" showAll="0">
       <items count="18">
         <item x="4"/>
         <item x="0"/>
@@ -10266,9 +10549,54 @@
     <field x="3"/>
     <field x="4"/>
   </rowFields>
-  <rowItems count="21">
+  <rowItems count="86">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
     <i>
       <x v="1"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="3"/>
     </i>
     <i r="1">
       <x/>
@@ -10298,7 +10626,142 @@
       <x v="3"/>
     </i>
     <i>
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i>
       <x v="8"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="14"/>
     </i>
     <i r="1">
       <x/>
@@ -10327,6 +10790,21 @@
     <i r="1">
       <x v="3"/>
     </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
     <i t="grand">
       <x/>
     </i>
@@ -10337,7 +10815,7 @@
   <dataFields count="1">
     <dataField name="Count of Order Number" fld="1" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
-  <chartFormats count="5">
+  <chartFormats count="7">
     <chartFormat chart="0" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
@@ -10383,19 +10861,26 @@
         </references>
       </pivotArea>
     </chartFormat>
+    <chartFormat chart="5" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="6" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
   </chartFormats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <filters count="1">
-    <filter fld="3" type="valueGreaterThan" evalOrder="-1" id="2" iMeasureFld="0">
-      <autoFilter ref="A1">
-        <filterColumn colId="0">
-          <customFilters>
-            <customFilter operator="greaterThan" val="40"/>
-          </customFilters>
-        </filterColumn>
-      </autoFilter>
-    </filter>
-  </filters>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
@@ -10408,7 +10893,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CA3CEB4E-A11A-2145-9D90-5FA49FD27D15}" name="PivotTable3" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CA3CEB4E-A11A-2145-9D90-5FA49FD27D15}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField axis="axisRow" showAll="0">
@@ -10932,15 +11417,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30FAE1F2-E552-BE40-ADDD-564FC7A126BA}">
-  <dimension ref="A3:B24"/>
+  <dimension ref="A3:B89"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q31" sqref="Q31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.83203125" bestFit="1" customWidth="1"/>
@@ -10958,10 +11443,10 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B4" s="4">
-        <v>46</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -10969,7 +11454,7 @@
         <v>21</v>
       </c>
       <c r="B5" s="4">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -10977,7 +11462,7 @@
         <v>19</v>
       </c>
       <c r="B6" s="4">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -10985,7 +11470,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="4">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -10993,12 +11478,12 @@
         <v>22</v>
       </c>
       <c r="B8" s="4">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B9" s="4">
         <v>46</v>
@@ -11009,7 +11494,7 @@
         <v>21</v>
       </c>
       <c r="B10" s="4">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -11017,7 +11502,7 @@
         <v>19</v>
       </c>
       <c r="B11" s="4">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -11025,7 +11510,7 @@
         <v>20</v>
       </c>
       <c r="B12" s="4">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -11033,15 +11518,15 @@
         <v>22</v>
       </c>
       <c r="B13" s="4">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B14" s="4">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -11049,7 +11534,7 @@
         <v>21</v>
       </c>
       <c r="B15" s="4">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -11057,7 +11542,7 @@
         <v>19</v>
       </c>
       <c r="B16" s="4">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -11065,7 +11550,7 @@
         <v>20</v>
       </c>
       <c r="B17" s="4">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -11073,15 +11558,15 @@
         <v>22</v>
       </c>
       <c r="B18" s="4">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B19" s="4">
-        <v>45</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -11089,7 +11574,7 @@
         <v>21</v>
       </c>
       <c r="B20" s="4">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -11097,7 +11582,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="4">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -11105,7 +11590,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="4">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -11113,15 +11598,535 @@
         <v>22</v>
       </c>
       <c r="B23" s="4">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="4">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" s="4">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B30" s="4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31" s="4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B32" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B33" s="4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B35" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B36" s="4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B37" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B38" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B39" s="4">
         <v>29</v>
       </c>
-      <c r="B24" s="4">
-        <v>181</v>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B40" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B41" s="4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B42" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B43" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B44" s="4">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B45" s="4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B46" s="4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B47" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B48" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B49" s="4">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B50" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B51" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B52" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B53" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B54" s="4">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B55" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B56" s="4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B57" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B58" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B59" s="4">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B60" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B61" s="4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B62" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B63" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B64" s="4">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B65" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B66" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B67" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B68" s="4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B69" s="4">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B70" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B71" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B72" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B73" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B74" s="4">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B75" s="4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B76" s="4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B77" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B78" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B79" s="4">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B80" s="4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B81" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B82" s="4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B83" s="4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B84" s="4">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B85" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B86" s="4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B87" s="4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B88" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B89" s="4">
+        <v>600</v>
       </c>
     </row>
   </sheetData>
@@ -11217,7 +12222,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H601"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>

</xml_diff>